<commit_message>
draft 1 of ms
</commit_message>
<xml_diff>
--- a/sarah_excel.xlsx
+++ b/sarah_excel.xlsx
@@ -8,29 +8,39 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f8d6885615144605/Documents/Duncan_Lab_2018/NHANES_WeightPerception/NHANES_wt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="244" documentId="11_5CC511A39121E779FCC6E9A5E66ADA9B43570D47" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{60B9E8E9-69C0-40A7-AA8E-0DF8C1A66246}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{7BCB5CFF-66B2-42B1-8701-A737A8D2AAA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3443" yWindow="0" windowWidth="19057" windowHeight="13147" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1410" yWindow="1410" windowWidth="18555" windowHeight="11827" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="05-13" sheetId="10" r:id="rId1"/>
-    <sheet name="FewerWaves" sheetId="9" r:id="rId2"/>
-    <sheet name="MainRes" sheetId="3" r:id="rId3"/>
-    <sheet name="SexStratified" sheetId="2" r:id="rId4"/>
-    <sheet name="RaceStratified" sheetId="8" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
+    <sheet name="tableone" sheetId="11" r:id="rId2"/>
+    <sheet name="polychoric" sheetId="12" r:id="rId3"/>
+    <sheet name="FewerWaves" sheetId="9" r:id="rId4"/>
+    <sheet name="MainRes" sheetId="3" r:id="rId5"/>
+    <sheet name="SexStratified" sheetId="2" r:id="rId6"/>
+    <sheet name="RaceStratified" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="734">
   <si>
     <t>Model 2 OR (95% CI)</t>
   </si>
@@ -1674,13 +1684,694 @@
   </si>
   <si>
     <t>1.47 (1.20 - 1.79)</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>&lt;0.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  2351517.8 ( 1.6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  999573.4 ( 2.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 45166674.4 (31.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12086805.8 (27.2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 48458478.2 (33.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13309647.2 (30.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 28494390.5 (19.6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9224626.6 (20.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12365652.6 ( 8.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4679972.6 (10.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  8605681.4 ( 5.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4104155.2 ( 9.2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 72861206.4 (49.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">21257593.7 (47.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">105188374.0 (71.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20976721.6 (46.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14374396.9 ( 9.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8587072.6 (19.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16067368.1 (11.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12343858.7 (27.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11056926.4 ( 7.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3031600.9 ( 6.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17279782.6 (12.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13677904.7 (31.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29961289.0 (20.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12069550.5 (27.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 97306810.7 (67.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17895028.7 (41.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 30982649.3 (21.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13844236.2 (30.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29241886.7 (19.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10421939.5 (23.2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 33466048.3 (22.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9947078.3 (22.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 32932577.7 (22.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7426344.5 (16.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20063903.5 (13.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3299655.4 ( 7.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  7295262.1 ( 5.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6800156.3 (15.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   About Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 58071563.0 (39.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17113618.7 (38.2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Overweight</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 82702484.2 (56.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">24459982.9 (54.6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Underweight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  5539571.7 ( 3.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3213919.7 ( 7.2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Same</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 38944031.3 (26.6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11987636.5 (26.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Less</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 99011750.9 (67.6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">27942773.0 (62.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   More</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  8457686.0 ( 5.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4915365.8 (11.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20535157.4 (15.6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6469119.0 (16.2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  5069834.6 ( 3.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3523494.9 ( 8.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 49932942.6 (37.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13220858.3 (33.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12246684.9 ( 9.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2426630.8 ( 6.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 44176900.0 (33.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14387697.1 (35.9) </t>
+  </si>
+  <si>
+    <t>Food Secure</t>
+  </si>
+  <si>
+    <t>Food Insecure</t>
+  </si>
+  <si>
+    <t>BMI category</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>Underweight</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Overweight</t>
+  </si>
+  <si>
+    <t>Obese (Class I)</t>
+  </si>
+  <si>
+    <t>Obese (Class II)</t>
+  </si>
+  <si>
+    <t>Obese (Class III)</t>
+  </si>
+  <si>
+    <t>Hispanic</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>High School Degree or Less</t>
+  </si>
+  <si>
+    <t>Some College</t>
+  </si>
+  <si>
+    <t>College Degree or Higher</t>
+  </si>
+  <si>
+    <t>Age Category</t>
+  </si>
+  <si>
+    <t>18 - 29</t>
+  </si>
+  <si>
+    <t>30 - 39</t>
+  </si>
+  <si>
+    <t>40 - 49</t>
+  </si>
+  <si>
+    <t>50 - 59</t>
+  </si>
+  <si>
+    <t>60 +</t>
+  </si>
+  <si>
+    <t>Depression</t>
+  </si>
+  <si>
+    <t>Weight Consideration</t>
+  </si>
+  <si>
+    <t>Like To Weigh</t>
+  </si>
+  <si>
+    <t>Not Doing Anything</t>
+  </si>
+  <si>
+    <t>Weighted for Survey Design</t>
+  </si>
+  <si>
+    <t>44939253.8 (23.4)</t>
+  </si>
+  <si>
+    <t>146687065.5 (76.6)</t>
+  </si>
+  <si>
+    <t>n (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  264 ( 1.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 149 ( 2.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4644 (30.2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1872 (26.2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5065 (33.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2179 (30.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3052 (19.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1537 (21.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1369 ( 8.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 749 (10.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  972 ( 6.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 666 ( 9.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7644 (49.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3361 (46.4) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6963 (44.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2177 (30.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3276 (21.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1885 (26.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3484 (22.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2679 (37.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1793 (11.6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 507 ( 7.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2800 (18.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2630 (37.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3170 (20.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1829 (26.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9187 (60.6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2498 (35.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3340 (21.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2075 (28.6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3127 (20.2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1564 (21.6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3224 (20.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1487 (20.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3032 (19.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1219 (16.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2793 (18.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 903 (12.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  918 ( 5.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1060 (14.6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6421 (41.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2881 (39.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8371 (54.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3822 (52.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  676 ( 4.4) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 516 ( 7.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4552 (29.4) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2096 (29.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9860 (63.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4344 (60.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1075 ( 6.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 795 (11.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2045 (14.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1028 (15.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  662 ( 4.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 571 ( 8.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4973 (36.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2076 (32.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1149 ( 8.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 378 ( 5.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4954 (35.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2433 (37.5) </t>
+  </si>
+  <si>
+    <t>Unweighted</t>
+  </si>
+  <si>
+    <t>7248 (31.8)</t>
+  </si>
+  <si>
+    <t>15516 (68.2)</t>
+  </si>
+  <si>
+    <t>Weight Perception</t>
+  </si>
+  <si>
+    <t>Desired Weight</t>
+  </si>
+  <si>
+    <t>Weight Action</t>
+  </si>
+  <si>
+    <t>BMI Category</t>
+  </si>
+  <si>
+    <r>
+      <t>0.080 (0.009)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>***</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>-0.307 (0.007)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>***</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>-0.897 (0.002)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>***</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>-0.354 (0.008)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>***</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.756 (0.004)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>***</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>-0.048 (0.010)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>***</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.417 (0.008)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>***</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>-0.712 (0.005)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>***</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.084 (0.010)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>***</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>-0.021 (0.010)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>***</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt; 0.001</t>
+  </si>
+  <si>
+    <t>Percent of sample</t>
+  </si>
+  <si>
+    <t>Normal Weight</t>
+  </si>
+  <si>
+    <t>Obesity (Class I)</t>
+  </si>
+  <si>
+    <t>Obesity (Class II)</t>
+  </si>
+  <si>
+    <t>Obesity (Class III)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1690,6 +2381,34 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1726,7 +2445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1761,6 +2480,59 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2046,8 +2818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E215E-8E74-4DA5-BF8B-BF6C691B1879}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2088,20 +2860,20 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="17" t="s">
         <v>2</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -2120,14 +2892,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+    <row r="5" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A5" s="18" t="s">
+        <v>641</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
       <c r="H5" t="s">
         <v>12</v>
       </c>
@@ -2136,21 +2908,21 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>419</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>429</v>
+    <row r="6" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>424</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>432</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>433</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>13</v>
@@ -2168,21 +2940,21 @@
         <v>483</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>412</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>420</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>437</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>428</v>
+    <row r="7" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A7" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>376</v>
       </c>
       <c r="F7" s="6"/>
       <c r="H7" s="2" t="s">
@@ -2201,22 +2973,14 @@
         <v>482</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>413</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>427</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>427</v>
-      </c>
+    <row r="8" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A8" s="18" t="s">
+        <v>715</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
       <c r="H8" s="2" t="s">
         <v>15</v>
       </c>
@@ -2233,21 +2997,21 @@
         <v>481</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>414</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>421</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>436</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>426</v>
+    <row r="9" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>431</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>434</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>16</v>
@@ -2265,14 +3029,22 @@
         <v>480</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+    <row r="10" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A10" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>416</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>423</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>435</v>
+      </c>
       <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
@@ -2281,22 +3053,14 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>415</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>422</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>431</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>434</v>
-      </c>
+    <row r="11" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A11" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
       <c r="H11" s="2" t="s">
         <v>18</v>
       </c>
@@ -2313,21 +3077,21 @@
         <v>491</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>416</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>423</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>430</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>435</v>
+    <row r="12" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A12" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>419</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>438</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>429</v>
       </c>
       <c r="F12" s="6"/>
       <c r="H12" s="2" t="s">
@@ -2346,14 +3110,22 @@
         <v>490</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+    <row r="13" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A13" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>412</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>420</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>437</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>428</v>
+      </c>
       <c r="H13" s="3" t="s">
         <v>20</v>
       </c>
@@ -2362,21 +3134,21 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>417</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>424</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>432</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>433</v>
+    <row r="14" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A14" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>413</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>427</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>427</v>
       </c>
       <c r="F14" s="6"/>
       <c r="H14" s="2" t="s">
@@ -2395,21 +3167,21 @@
         <v>498</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>425</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>376</v>
+    <row r="15" spans="1:12" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>414</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>436</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>426</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>22</v>
@@ -2427,9 +3199,14 @@
         <v>497</v>
       </c>
     </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>275</v>
       </c>
       <c r="H18" t="s">
         <v>6</v>
@@ -2437,7 +3214,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H19" t="s">
         <v>275</v>
@@ -2445,52 +3222,62 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H20" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>277</v>
-      </c>
       <c r="H21" t="s">
         <v>277</v>
       </c>
     </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>459</v>
+      </c>
+    </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>459</v>
-      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B25" s="4"/>
-      <c r="C25" s="9"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>457</v>
+      </c>
       <c r="D25" s="13"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A26" s="1"/>
-      <c r="B26" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>457</v>
-      </c>
+      <c r="A26" t="s">
+        <v>227</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="13"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>227</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="9"/>
+      <c r="A27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="6"/>
       <c r="F27" s="9"/>
       <c r="H27" s="1" t="s">
         <v>352</v>
@@ -2502,30 +3289,25 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>462</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>466</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="6"/>
+      <c r="A29" t="s">
+        <v>228</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="H29" t="s">
         <v>318</v>
@@ -2536,12 +3318,17 @@
       <c r="L29" s="4"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>228</v>
-      </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="A30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="6"/>
       <c r="F30" s="4"/>
       <c r="H30" s="1" t="s">
         <v>11</v>
@@ -2561,16 +3348,16 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>461</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>112</v>
+        <v>19</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>465</v>
       </c>
       <c r="D31" s="2"/>
-      <c r="E31" s="6"/>
+      <c r="E31" s="4"/>
       <c r="F31" s="6"/>
       <c r="H31" t="s">
         <v>12</v>
@@ -2581,16 +3368,8 @@
       <c r="L31" s="4"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>460</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>465</v>
-      </c>
-      <c r="D32" s="2"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="7"/>
       <c r="H32" s="2" t="s">
@@ -2610,8 +3389,13 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>239</v>
+      </c>
       <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>458</v>
+      </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="H33" s="2" t="s">
@@ -2631,13 +3415,8 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>239</v>
-      </c>
       <c r="B34" s="4"/>
-      <c r="C34" s="4" t="s">
-        <v>458</v>
-      </c>
+      <c r="C34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="H34" s="2" t="s">
@@ -2657,9 +3436,6 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="H35" s="2" t="s">
         <v>16</v>
@@ -2687,6 +3463,9 @@
       <c r="L36" s="4"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>439</v>
+      </c>
       <c r="H37" s="2" t="s">
         <v>18</v>
       </c>
@@ -2705,7 +3484,13 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>439</v>
+        <v>198</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>457</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>19</v>
@@ -2724,15 +3509,16 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>198</v>
+      <c r="A39" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>457</v>
-      </c>
+        <v>447</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="D39" s="2"/>
       <c r="H39" s="3" t="s">
         <v>20</v>
       </c>
@@ -2743,13 +3529,13 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>451</v>
+        <v>14</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>450</v>
       </c>
       <c r="D40" s="2"/>
       <c r="H40" s="2" t="s">
@@ -2770,13 +3556,13 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D41" s="2"/>
       <c r="H41" s="2" t="s">
@@ -2797,47 +3583,47 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>445</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>449</v>
+        <v>16</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>448</v>
       </c>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A43" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="D43" s="2"/>
+      <c r="A43" t="s">
+        <v>440</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>440</v>
-      </c>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
+      <c r="A44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="D44" s="2"/>
       <c r="H44" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>455</v>
+        <v>14</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>454</v>
       </c>
       <c r="D45" s="2"/>
       <c r="H45" t="s">
@@ -2846,13 +3632,13 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>443</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>454</v>
+        <v>15</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>453</v>
       </c>
       <c r="D46" s="2"/>
       <c r="H46" t="s">
@@ -2861,40 +3647,28 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D47" s="2"/>
       <c r="H47" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A48" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="D48" s="2"/>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A49" s="2"/>
+      <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A50" s="2"/>
-      <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+      <c r="A50" t="s">
         <v>212</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C50" t="s">
         <v>458</v>
       </c>
     </row>
@@ -3117,10 +3891,1215 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F53FCF18-65A6-470F-B64B-661057994B28}">
+  <dimension ref="A1:L49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="24.265625" customWidth="1"/>
+    <col min="2" max="2" width="23.796875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="23.1328125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="7.73046875" style="15" customWidth="1"/>
+    <col min="5" max="5" width="17.1328125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="19.796875" style="15" customWidth="1"/>
+    <col min="7" max="7" width="9.06640625" style="15"/>
+    <col min="9" max="9" width="24.265625" customWidth="1"/>
+    <col min="10" max="10" width="12.1328125" style="15" customWidth="1"/>
+    <col min="11" max="11" width="11.59765625" style="15" customWidth="1"/>
+    <col min="12" max="12" width="7.73046875" style="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B1" s="32" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="E1" s="33" t="s">
+        <v>711</v>
+      </c>
+      <c r="F1" s="33"/>
+      <c r="J1" s="32" t="s">
+        <v>644</v>
+      </c>
+      <c r="K1" s="32"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B2" s="15" t="s">
+        <v>618</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>619</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>619</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="30" t="s">
+        <v>618</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>619</v>
+      </c>
+      <c r="L2" s="31" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>647</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>646</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>645</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>713</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>712</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>729</v>
+      </c>
+      <c r="J3" s="29">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="K3" s="29">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>620</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="I4" t="s">
+        <v>620</v>
+      </c>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="15" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>550</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>551</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>649</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>650</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="J5" s="29">
+        <v>1.6</v>
+      </c>
+      <c r="K5" s="29">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>552</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>553</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>651</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>652</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="J6" s="29">
+        <v>31.1</v>
+      </c>
+      <c r="K6" s="29">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>554</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>555</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>653</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>654</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="J7" s="29">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="K7" s="29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>556</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>557</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>655</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>656</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="J8" s="29">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="K8" s="29">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>558</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>559</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>657</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>658</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="J9" s="29">
+        <v>8.5</v>
+      </c>
+      <c r="K9" s="29">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>560</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>659</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>660</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="J10" s="29">
+        <v>5.9</v>
+      </c>
+      <c r="K10" s="29">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" s="2"/>
+      <c r="I11" t="s">
+        <v>228</v>
+      </c>
+      <c r="J11" s="29">
+        <v>49.7</v>
+      </c>
+      <c r="K11" s="29">
+        <v>47.3</v>
+      </c>
+      <c r="L11" s="15">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>228</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>562</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>563</v>
+      </c>
+      <c r="D12" s="15">
+        <v>2E-3</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>661</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>662</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="I12" t="s">
+        <v>621</v>
+      </c>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="15" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I13" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="J13" s="29">
+        <v>71.7</v>
+      </c>
+      <c r="K13" s="29">
+        <v>46.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>621</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="J14" s="29">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="K14" s="29">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>564</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>565</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>663</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>664</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="J15" s="29">
+        <v>11</v>
+      </c>
+      <c r="K15" s="29">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>567</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>665</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>666</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="J16" s="29">
+        <v>7.5</v>
+      </c>
+      <c r="K16" s="29">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>568</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>569</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>667</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>668</v>
+      </c>
+      <c r="I17" t="s">
+        <v>630</v>
+      </c>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="15" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>570</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>571</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>669</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>670</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="J18" s="29">
+        <v>12</v>
+      </c>
+      <c r="K18" s="29">
+        <v>31.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="J19" s="29">
+        <v>20.7</v>
+      </c>
+      <c r="K19" s="29">
+        <v>27.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>630</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="J20" s="29">
+        <v>67.3</v>
+      </c>
+      <c r="K20" s="29">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>572</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>573</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>671</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>672</v>
+      </c>
+      <c r="I21" t="s">
+        <v>634</v>
+      </c>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="15" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>574</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>575</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>674</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="J22" s="29">
+        <v>21.1</v>
+      </c>
+      <c r="K22" s="29">
+        <v>30.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>576</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>577</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>675</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>676</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="J23" s="29">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="K23" s="29">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A24" s="2"/>
+      <c r="I24" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="J24" s="29">
+        <v>22.8</v>
+      </c>
+      <c r="K24" s="29">
+        <v>22.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>634</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="J25" s="29">
+        <v>22.5</v>
+      </c>
+      <c r="K25" s="29">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>578</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>579</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>677</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>678</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="J26" s="29">
+        <v>13.7</v>
+      </c>
+      <c r="K26" s="29">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>580</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>581</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>679</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>680</v>
+      </c>
+      <c r="I27" t="s">
+        <v>640</v>
+      </c>
+      <c r="J27" s="29">
+        <v>5</v>
+      </c>
+      <c r="K27" s="29">
+        <v>15.1</v>
+      </c>
+      <c r="L27" s="15" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A28" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>582</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>583</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>681</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>682</v>
+      </c>
+      <c r="I28" t="s">
+        <v>641</v>
+      </c>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="15" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>584</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>585</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>683</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>684</v>
+      </c>
+      <c r="I29" t="s">
+        <v>590</v>
+      </c>
+      <c r="J29" s="29">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="K29" s="29">
+        <v>38.200000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>586</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>587</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>685</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>686</v>
+      </c>
+      <c r="I30" t="s">
+        <v>593</v>
+      </c>
+      <c r="J30" s="29">
+        <v>56.5</v>
+      </c>
+      <c r="K30" s="29">
+        <v>54.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I31" t="s">
+        <v>596</v>
+      </c>
+      <c r="J31" s="29">
+        <v>3.8</v>
+      </c>
+      <c r="K31" s="29">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>640</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>588</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>589</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>687</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>688</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="I32" t="s">
+        <v>642</v>
+      </c>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="15" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I33" t="s">
+        <v>599</v>
+      </c>
+      <c r="J33" s="29">
+        <v>26.6</v>
+      </c>
+      <c r="K33" s="29">
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>641</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="I34" t="s">
+        <v>602</v>
+      </c>
+      <c r="J34" s="29">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="K34" s="29">
+        <v>62.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>590</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>591</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>592</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>689</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>690</v>
+      </c>
+      <c r="I35" t="s">
+        <v>605</v>
+      </c>
+      <c r="J35" s="29">
+        <v>5.8</v>
+      </c>
+      <c r="K35" s="29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>593</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>594</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>595</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>691</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>692</v>
+      </c>
+      <c r="I36" t="s">
+        <v>12</v>
+      </c>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="15" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>596</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>597</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>598</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>693</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>694</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" s="29">
+        <v>15.6</v>
+      </c>
+      <c r="K37" s="29">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="29">
+        <v>3.8</v>
+      </c>
+      <c r="K38" s="29">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>642</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39" s="29">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="K39" s="29">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>599</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>600</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>601</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>695</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>696</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J40" s="29">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="K40" s="29">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>602</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>603</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>604</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>697</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>698</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="J41" s="29">
+        <v>33.5</v>
+      </c>
+      <c r="K41" s="29">
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>605</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>607</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>699</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="G44" s="15" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>608</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>609</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>701</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>611</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>703</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>612</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>613</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>705</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A48" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>614</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>615</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>707</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>616</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>617</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>709</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>710</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7B9394-496E-4EE1-BD07-23DAC7C48C6A}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.4" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.46484375" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.46484375" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.265625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="15.06640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.06640625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="16"/>
+      <c r="B1" s="25" t="s">
+        <v>717</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>714</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>715</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="A2" s="26" t="s">
+        <v>309</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>718</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>723</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>726</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="A3" s="26" t="s">
+        <v>717</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>722</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>725</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="A4" s="26" t="s">
+        <v>714</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>720</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="A5" s="27" t="s">
+        <v>715</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>385</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>385</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>724</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
@@ -4094,7 +6073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
@@ -4702,12 +6681,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection sqref="A1:I11"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4992,7 +6971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
@@ -5228,7 +7207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>

</xml_diff>